<commit_message>
Se actualizan mediciones de rendimiento y grafica, ademas se añaden fotos de evidencia
</commit_message>
<xml_diff>
--- a/Proyecto2.2/desing/medicionesDeRendimiento.xlsx
+++ b/Proyecto2.2/desing/medicionesDeRendimiento.xlsx
@@ -5,125 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\Documents\UCR\II SEMESTRE 2022\Paralela\PROYECTO\stack_overfloismo\Proyecto2.2\desing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ufonseca\Documents\PersonalUFH\PARALELA\stack_overfloismo\Proyecto2.2\desing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98361B74-3307-43BE-8821-762D23DDEABE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D8C5D3-C5B4-4AEE-A797-0302B26912CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proy02" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-    <author>Allan Berrocal</author>
-  </authors>
-  <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Liberation Sans1"/>
-          </rPr>
-          <t>Number of available CPUs in the test machine</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Liberation Sans1"/>
-          </rPr>
-          <t>Serial</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Liberation Sans1"/>
-          </rPr>
-          <t>Default block mapping (static)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Liberation Sans1"/>
-          </rPr>
-          <t>Cyclic mapping (static,1)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{7715078B-04B0-40B0-95A0-FAE115E1EA76}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
-            <rFont val="Liberation Sans1"/>
-          </rPr>
-          <t>Type the test case used to measure the performance</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{8DF4F505-F3CB-4395-8E7C-6BA488C8C21F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Liberation Sans1"/>
-          </rPr>
-          <t>Duration in seconds running with no thread support (main thread calculates everything)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{48CA40E7-8285-4C3B-A40B-7B97FFE6B504}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Liberation Sans1"/>
-          </rPr>
-          <t>Type formula here to calculate the speedup relative to the serial version</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{2AEAF5C4-35C3-4367-8E53-AADDEDF111AD}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Liberation Sans1"/>
-          </rPr>
-          <t>Type formula here to calculate the efficiency relative to the serial version</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -153,9 +46,6 @@
     <t>Distributed</t>
   </si>
   <si>
-    <t>job001.txt</t>
-  </si>
-  <si>
     <t>Processes</t>
   </si>
   <si>
@@ -167,15 +57,19 @@
   <si>
     <t>Hybrid</t>
   </si>
+  <si>
+    <t>job003.txt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$₡-140A]&quot; &quot;#,##0.00;[Red]&quot;-&quot;[$₡-140A]&quot; &quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -247,11 +141,6 @@
       <i/>
       <u/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Liberation Sans1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Liberation Sans1"/>
     </font>
@@ -441,7 +330,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -449,19 +338,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -473,14 +359,23 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -603,10 +498,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64640883977900554</c:v>
+                  <c:v>0.43739784243216745</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.80689655172413788</c:v>
+                  <c:v>1.0007479431563202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -692,14 +587,14 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.000">
                   <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64640883977900554</c:v>
+                  <c:v>0.43739784243216745</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.10086206896551723</c:v>
+                <c:pt idx="2" formatCode="0.000">
+                  <c:v>0.12509349289454003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1027,7 +922,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2618,24 +2513,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="1023" width="7.21875" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="8.36328125" customWidth="1"/>
+    <col min="9" max="1023" width="7.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2643,42 +2538,42 @@
       <c r="C1" s="2">
         <v>8</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:8" ht="15.6">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75">
+    <row r="3" spans="1:8" ht="15.6">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="8">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E3" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75">
+    <row r="4" spans="1:8" ht="15.6">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2697,55 +2592,55 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="15" t="s">
-        <v>8</v>
+      <c r="A5" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="9">
-        <v>117</v>
-      </c>
-      <c r="D5" s="11">
-        <v>181</v>
-      </c>
-      <c r="E5" s="11">
-        <v>145</v>
+      <c r="C5" s="15">
+        <v>133.80000000000001</v>
+      </c>
+      <c r="D5" s="10">
+        <v>305.89999999999998</v>
+      </c>
+      <c r="E5" s="10">
+        <v>133.69999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="15"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <f>C5/D5</f>
-        <v>0.64640883977900554</v>
-      </c>
-      <c r="E6" s="12">
+        <v>0.43739784243216745</v>
+      </c>
+      <c r="E6" s="11">
         <f>C5/E5</f>
-        <v>0.80689655172413788</v>
+        <v>1.0007479431563202</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="15"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="16">
         <f>C6/C4</f>
         <v>0.125</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <f>D6/D4</f>
-        <v>0.64640883977900554</v>
-      </c>
-      <c r="E7" s="12">
+        <v>0.43739784243216745</v>
+      </c>
+      <c r="E7" s="17">
         <f>E6/E4</f>
-        <v>0.10086206896551723</v>
+        <v>0.12509349289454003</v>
       </c>
       <c r="H7" s="6"/>
     </row>
@@ -2761,6 +2656,5 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>